<commit_message>
document of virtualenv added and work-log updated
</commit_message>
<xml_diff>
--- a/Docs/pip cmd.xlsx
+++ b/Docs/pip cmd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>COMMANDS</t>
   </si>
@@ -118,6 +118,63 @@
   </si>
   <si>
     <t>it will upload the distribution to PyPI</t>
+  </si>
+  <si>
+    <t>pip install virtualenv</t>
+  </si>
+  <si>
+    <t>it will create a virtual environment</t>
+  </si>
+  <si>
+    <t>virtualenv --version</t>
+  </si>
+  <si>
+    <t>it show the version of virtualen</t>
+  </si>
+  <si>
+    <t>virtualenv MyProject</t>
+  </si>
+  <si>
+    <t>it will a virtualenv for MyProject</t>
+  </si>
+  <si>
+    <t>cd/source/MyProject/Scripts/activate.bat</t>
+  </si>
+  <si>
+    <t>it will activate the virualenv</t>
+  </si>
+  <si>
+    <t>deactivate</t>
+  </si>
+  <si>
+    <t>it will deactivate the virtual env</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> virtualenv --no-site-packages </t>
+  </si>
+  <si>
+    <t>it will not include the packages that are installed globally</t>
+  </si>
+  <si>
+    <t>pip install virtualenvwrapper</t>
+  </si>
+  <si>
+    <t>it will install virtualen wrapper</t>
+  </si>
+  <si>
+    <t>mkvirtualenv my_project</t>
+  </si>
+  <si>
+    <t>workon my_project</t>
+  </si>
+  <si>
+    <t>it will enable u to work on that project</t>
+  </si>
+  <si>
+    <t>rmvirtualenv venv</t>
+  </si>
+  <si>
+    <t>it will remov/delete the virtualenv</t>
   </si>
 </sst>
 </file>
@@ -521,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -668,6 +725,94 @@
       </c>
       <c r="B17" s="5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>